<commit_message>
Progress on comput. benchmarks
</commit_message>
<xml_diff>
--- a/Configuration/ITER_1D.xlsx
+++ b/Configuration/ITER_1D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laghi\Documents\03_dottorato\04_F4E\01_JADE\Code\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BE4BC9-E3F7-4CCD-A72C-163E7FB53907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18E3DEF-47F5-4DC9-B65D-C220488192DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2FBD261-A6D7-48D0-8F16-20EC1D949C31}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B2FBD261-A6D7-48D0-8F16-20EC1D949C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="26">
   <si>
     <t>Tally</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,11 +213,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -226,6 +232,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,406 +558,406 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3790D3-7F45-4640-BF40-10D0C8032039}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="14" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="6"/>
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>34</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>44</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>54</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>64</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>74</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>84</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>94</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>104</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>114</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>124</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>134</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>144</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>154</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>164</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>174</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="7">
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -968,140 +983,197 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6571A1-07E0-421E-984F-64E4648982CB}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="14.44140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="9">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="9">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>6</v>
+      <c r="A4" s="9">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="9">
         <v>16</v>
       </c>
+      <c r="B5" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="9">
         <v>26</v>
       </c>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="9">
         <v>24</v>
       </c>
+      <c r="B7" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="9">
         <v>34</v>
       </c>
+      <c r="B8" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="9">
         <v>44</v>
       </c>
+      <c r="B9" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="9">
         <v>54</v>
       </c>
+      <c r="B10" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="9">
         <v>64</v>
       </c>
+      <c r="B11" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="9">
         <v>74</v>
       </c>
+      <c r="B12" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="9">
         <v>84</v>
       </c>
+      <c r="B13" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="9">
         <v>94</v>
       </c>
+      <c r="B14" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="9">
         <v>104</v>
       </c>
+      <c r="B15" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="9">
         <v>114</v>
       </c>
+      <c r="B16" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="9">
         <v>124</v>
       </c>
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="9">
         <v>134</v>
       </c>
+      <c r="B18" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="9">
         <v>144</v>
       </c>
+      <c r="B19" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="9">
         <v>154</v>
       </c>
+      <c r="B20" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="9">
         <v>164</v>
       </c>
+      <c r="B21" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="9">
         <v>174</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="9" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1119,67 +1191,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>